<commit_message>
generated figures for nsf  report
</commit_message>
<xml_diff>
--- a/time_series_analysis/Figures/Environmental/temp_metric_table_ms.xlsx
+++ b/time_series_analysis/Figures/Environmental/temp_metric_table_ms.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/E5/timeseries/time_series_analysis/Figures/Environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827EA040-7611-F744-B098-7BEE2CC1BDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A67434-999A-5F4B-A4EA-0B450111124C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31320" yWindow="100" windowWidth="26700" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="temp_metric_table" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">temp_metric_table!$B$2:$F$10</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -59,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,6 +206,19 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -745,29 +761,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1127,7 +1143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="170" zoomScaleNormal="180" zoomScalePageLayoutView="170" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="270" zoomScaleNormal="180" zoomScalePageLayoutView="270" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1138,144 +1156,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="8">
         <v>28.987320707070701</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="9">
         <v>28.713333333333299</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="10">
         <v>28.772285984848502</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="9">
         <v>28.208254009599099</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="8">
         <v>28.284273843125</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="10">
         <v>28.215426272061102</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19"/>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="8">
         <v>1.2688573232323199</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="9">
         <v>0.72336488340192096</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="10">
         <v>0.93610101010100599</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="20"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <v>0.34588612015447801</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <v>0.201604114155956</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="14">
         <v>0.268546758953501</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="8">
         <v>31.331111111111099</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="9">
         <v>30.95</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="10">
         <v>30.747777777777799</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19"/>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="8">
         <v>28.326167947387798</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="9">
         <v>28.260120735269201</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="10">
         <v>28.2786447126418</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="8">
         <v>6.8472222222222001</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="9">
         <v>6.4420000000000002</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="10">
         <v>5.3677777777777997</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>0.95012740575139898</v>
       </c>
       <c r="E10" s="17">
         <v>0.84627488130421302</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="18">
         <v>0.90397696773215597</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated univariate figures, added posthoc tests, added model output
</commit_message>
<xml_diff>
--- a/time_series_analysis/Figures/Environmental/temp_metric_table_ms.xlsx
+++ b/time_series_analysis/Figures/Environmental/temp_metric_table_ms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/E5/timeseries/time_series_analysis/Figures/Environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A67434-999A-5F4B-A4EA-0B450111124C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBBD608-15C2-0B49-870C-0D3FA763A37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>SD</t>
   </si>
   <si>
-    <t>Timeseries</t>
+    <t>Annual</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1144,7 @@
   <dimension ref="B1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="270" zoomScaleNormal="180" zoomScalePageLayoutView="270" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>